<commit_message>
Added value prompt and pdf export
</commit_message>
<xml_diff>
--- a/qasaym_template.xlsx
+++ b/qasaym_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t xml:space="preserve">الجمله</t>
   </si>
@@ -711,59 +711,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:BB1048576"/>
+  <dimension ref="A1:BB36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AY35" activeCellId="0" sqref="A35:AY35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BB19" activeCellId="0" sqref="BB19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="35.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="86.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="14" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="29" style="0" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="39" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="15.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="16.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="25.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="1" style="0" width="18.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="29.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="55" style="0" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>960</v>
       </c>
@@ -982,13 +945,21 @@
       <c r="R2" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="S2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="U2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="V2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="X2" s="4" t="n">
         <v>0</v>
       </c>
@@ -1079,7 +1050,7 @@
       <c r="BA2" s="5"/>
       <c r="BB2" s="5"/>
     </row>
-    <row r="3" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>900</v>
       </c>
@@ -1134,13 +1105,21 @@
       <c r="R3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="S3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
+      <c r="V3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X3" s="5" t="n">
         <v>0</v>
       </c>
@@ -1231,7 +1210,7 @@
       <c r="BA3" s="5"/>
       <c r="BB3" s="5"/>
     </row>
-    <row r="4" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>900</v>
       </c>
@@ -1286,13 +1265,21 @@
       <c r="R4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="S4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
+      <c r="V4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X4" s="5" t="n">
         <v>0</v>
       </c>
@@ -1383,7 +1370,7 @@
       <c r="BA4" s="5"/>
       <c r="BB4" s="5"/>
     </row>
-    <row r="5" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>900</v>
       </c>
@@ -1438,13 +1425,21 @@
       <c r="R5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="S5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="V5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X5" s="5" t="n">
         <v>0</v>
       </c>
@@ -1535,7 +1530,7 @@
       <c r="BA5" s="5"/>
       <c r="BB5" s="5"/>
     </row>
-    <row r="6" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>900</v>
       </c>
@@ -1590,13 +1585,21 @@
       <c r="R6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="S6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
+      <c r="V6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X6" s="5" t="n">
         <v>0</v>
       </c>
@@ -1687,7 +1690,7 @@
       <c r="BA6" s="5"/>
       <c r="BB6" s="5"/>
     </row>
-    <row r="7" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>450</v>
       </c>
@@ -1742,13 +1745,21 @@
       <c r="R7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="S7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+      <c r="V7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X7" s="5" t="n">
         <v>0</v>
       </c>
@@ -1839,7 +1850,7 @@
       <c r="BA7" s="5"/>
       <c r="BB7" s="5"/>
     </row>
-    <row r="8" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>739.25</v>
       </c>
@@ -1855,12 +1866,24 @@
       <c r="E8" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="F8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L8" s="5" t="n">
         <v>0</v>
       </c>
@@ -1882,17 +1905,27 @@
       <c r="R8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="S8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
+      <c r="V8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y8" s="5"/>
+      <c r="Y8" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z8" s="5" t="n">
         <v>0</v>
       </c>
@@ -1977,7 +2010,7 @@
       <c r="BA8" s="5"/>
       <c r="BB8" s="5"/>
     </row>
-    <row r="9" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>739.25</v>
       </c>
@@ -1993,12 +2026,24 @@
       <c r="E9" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="F9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L9" s="5" t="n">
         <v>0</v>
       </c>
@@ -2020,17 +2065,27 @@
       <c r="R9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="S9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
+      <c r="V9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y9" s="5"/>
+      <c r="Y9" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z9" s="5" t="n">
         <v>0</v>
       </c>
@@ -2115,7 +2170,7 @@
       <c r="BA9" s="5"/>
       <c r="BB9" s="5"/>
     </row>
-    <row r="10" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>739.25</v>
       </c>
@@ -2131,12 +2186,24 @@
       <c r="E10" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L10" s="5" t="n">
         <v>0</v>
       </c>
@@ -2158,17 +2225,27 @@
       <c r="R10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="S10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="U10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
+      <c r="V10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="X10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y10" s="5"/>
+      <c r="Y10" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z10" s="5" t="n">
         <v>0</v>
       </c>
@@ -2253,7 +2330,7 @@
       <c r="BA10" s="5"/>
       <c r="BB10" s="5"/>
     </row>
-    <row r="11" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>100</v>
       </c>
@@ -2269,12 +2346,24 @@
       <c r="E11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="F11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L11" s="5" t="n">
         <v>0</v>
       </c>
@@ -2296,17 +2385,27 @@
       <c r="R11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="S11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
+      <c r="V11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y11" s="5"/>
+      <c r="Y11" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z11" s="5" t="n">
         <v>0</v>
       </c>
@@ -2391,7 +2490,7 @@
       <c r="BA11" s="5"/>
       <c r="BB11" s="5"/>
     </row>
-    <row r="12" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>64</v>
       </c>
@@ -2407,12 +2506,24 @@
       <c r="E12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L12" s="5" t="n">
         <v>0</v>
       </c>
@@ -2434,17 +2545,27 @@
       <c r="R12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="S12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
+      <c r="V12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y12" s="5"/>
+      <c r="Y12" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z12" s="5" t="n">
         <v>0</v>
       </c>
@@ -2529,7 +2650,7 @@
       <c r="BA12" s="5"/>
       <c r="BB12" s="5"/>
     </row>
-    <row r="13" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>64</v>
       </c>
@@ -2545,12 +2666,24 @@
       <c r="E13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L13" s="5" t="n">
         <v>0</v>
       </c>
@@ -2572,17 +2705,27 @@
       <c r="R13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="S13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
+      <c r="V13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y13" s="5"/>
+      <c r="Y13" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z13" s="5" t="n">
         <v>0</v>
       </c>
@@ -2667,7 +2810,7 @@
       <c r="BA13" s="5"/>
       <c r="BB13" s="5"/>
     </row>
-    <row r="14" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
@@ -2683,12 +2826,24 @@
       <c r="E14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="F14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L14" s="5" t="n">
         <v>0</v>
       </c>
@@ -2710,17 +2865,27 @@
       <c r="R14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
+      <c r="S14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
+      <c r="V14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y14" s="5"/>
+      <c r="Y14" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z14" s="5" t="n">
         <v>0</v>
       </c>
@@ -2805,7 +2970,7 @@
       <c r="BA14" s="5"/>
       <c r="BB14" s="5"/>
     </row>
-    <row r="15" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>3</v>
       </c>
@@ -2821,12 +2986,24 @@
       <c r="E15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="F15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L15" s="5" t="n">
         <v>0</v>
       </c>
@@ -2848,17 +3025,27 @@
       <c r="R15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="S15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
+      <c r="V15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y15" s="5"/>
+      <c r="Y15" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z15" s="5" t="n">
         <v>0</v>
       </c>
@@ -2943,7 +3130,7 @@
       <c r="BA15" s="5"/>
       <c r="BB15" s="5"/>
     </row>
-    <row r="16" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>80</v>
       </c>
@@ -2959,12 +3146,24 @@
       <c r="E16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L16" s="5" t="n">
         <v>0</v>
       </c>
@@ -2986,17 +3185,27 @@
       <c r="R16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="S16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
+      <c r="V16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y16" s="5"/>
+      <c r="Y16" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z16" s="5" t="n">
         <v>0</v>
       </c>
@@ -3081,7 +3290,7 @@
       <c r="BA16" s="5"/>
       <c r="BB16" s="5"/>
     </row>
-    <row r="17" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>696</v>
       </c>
@@ -3136,21 +3345,33 @@
       <c r="R17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="S17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
+      <c r="V17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y17" s="5"/>
+      <c r="Y17" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AA17" s="5"/>
+      <c r="AA17" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AB17" s="5" t="n">
         <v>0</v>
       </c>
@@ -3229,9 +3450,9 @@
       <c r="BA17" s="5"/>
       <c r="BB17" s="5"/>
     </row>
-    <row r="18" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>71</v>
+    <row r="18" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0</v>
@@ -3284,13 +3505,21 @@
       <c r="R18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="S18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="U18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
+      <c r="V18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="X18" s="5" t="n">
         <v>0</v>
       </c>
@@ -3381,9 +3610,9 @@
       <c r="BA18" s="5"/>
       <c r="BB18" s="5"/>
     </row>
-    <row r="19" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0</v>
@@ -3397,12 +3626,24 @@
       <c r="E19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="F19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L19" s="5" t="n">
         <v>0</v>
       </c>
@@ -3424,17 +3665,27 @@
       <c r="R19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="S19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
+      <c r="V19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y19" s="5"/>
+      <c r="Y19" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z19" s="5" t="n">
         <v>0</v>
       </c>
@@ -3519,7 +3770,7 @@
       <c r="BA19" s="5"/>
       <c r="BB19" s="5"/>
     </row>
-    <row r="20" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>0</v>
       </c>
@@ -3535,12 +3786,24 @@
       <c r="E20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="F20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L20" s="5" t="n">
         <v>0</v>
       </c>
@@ -3562,21 +3825,33 @@
       <c r="R20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="S20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
+      <c r="V20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y20" s="5"/>
+      <c r="Y20" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AA20" s="5"/>
+      <c r="AA20" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AB20" s="5" t="n">
         <v>0</v>
       </c>
@@ -3655,7 +3930,7 @@
       <c r="BA20" s="5"/>
       <c r="BB20" s="5"/>
     </row>
-    <row r="21" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>839.25</v>
       </c>
@@ -3710,13 +3985,21 @@
       <c r="R21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="S21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
+      <c r="V21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X21" s="5" t="n">
         <v>0</v>
       </c>
@@ -3807,7 +4090,7 @@
       <c r="BA21" s="5"/>
       <c r="BB21" s="5"/>
     </row>
-    <row r="22" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>1000</v>
       </c>
@@ -3862,13 +4145,21 @@
       <c r="R22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="S22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
+      <c r="V22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X22" s="5" t="n">
         <v>0</v>
       </c>
@@ -3959,8 +4250,10 @@
       <c r="BA22" s="5"/>
       <c r="BB22" s="5"/>
     </row>
-    <row r="23" s="6" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
+    <row r="23" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="B23" s="5" t="n">
         <v>0</v>
       </c>
@@ -4012,13 +4305,21 @@
       <c r="R23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="S23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
+      <c r="V23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X23" s="5" t="n">
         <v>0</v>
       </c>
@@ -4109,7 +4410,7 @@
       <c r="BA23" s="7"/>
       <c r="BB23" s="5"/>
     </row>
-    <row r="24" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>150</v>
       </c>
@@ -4164,13 +4465,21 @@
       <c r="R24" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="S24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U24" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
+      <c r="V24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X24" s="5" t="n">
         <v>0</v>
       </c>
@@ -4261,7 +4570,7 @@
       <c r="BA24" s="7"/>
       <c r="BB24" s="5"/>
     </row>
-    <row r="25" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
         <v>200</v>
       </c>
@@ -4316,13 +4625,21 @@
       <c r="R25" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="S25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U25" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
+      <c r="V25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X25" s="5" t="n">
         <v>0</v>
       </c>
@@ -4413,7 +4730,7 @@
       <c r="BA25" s="7"/>
       <c r="BB25" s="5"/>
     </row>
-    <row r="26" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>67</v>
       </c>
@@ -4429,12 +4746,24 @@
       <c r="E26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="F26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="L26" s="5" t="n">
         <v>0</v>
       </c>
@@ -4456,21 +4785,33 @@
       <c r="R26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
+      <c r="S26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
+      <c r="V26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y26" s="5"/>
+      <c r="Y26" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="Z26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AA26" s="5"/>
+      <c r="AA26" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AB26" s="5" t="n">
         <v>0</v>
       </c>
@@ -4549,7 +4890,7 @@
       <c r="BA26" s="5"/>
       <c r="BB26" s="5"/>
     </row>
-    <row r="27" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -4604,13 +4945,21 @@
       <c r="R27" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="S27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U27" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
+      <c r="V27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X27" s="5" t="n">
         <v>0</v>
       </c>
@@ -4620,7 +4969,9 @@
       <c r="Z27" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AA27" s="5"/>
+      <c r="AA27" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AB27" s="5" t="n">
         <v>0</v>
       </c>
@@ -4699,8 +5050,10 @@
       <c r="BA27" s="5"/>
       <c r="BB27" s="5"/>
     </row>
-    <row r="28" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
+    <row r="28" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
       </c>
@@ -4752,13 +5105,21 @@
       <c r="R28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="S28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
+      <c r="V28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X28" s="5" t="n">
         <v>0</v>
       </c>
@@ -4768,7 +5129,9 @@
       <c r="Z28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AA28" s="5"/>
+      <c r="AA28" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AB28" s="5" t="n">
         <v>0</v>
       </c>
@@ -4847,377 +5210,969 @@
       <c r="BA28" s="5"/>
       <c r="BB28" s="5"/>
     </row>
-    <row r="29" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+    <row r="29" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U29" s="5" t="n">
         <v>54</v>
       </c>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
+      <c r="V29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AG29" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5"/>
-      <c r="AL29" s="5"/>
-      <c r="AM29" s="5"/>
-      <c r="AN29" s="5"/>
-      <c r="AO29" s="5"/>
-      <c r="AP29" s="5"/>
-      <c r="AQ29" s="5"/>
-      <c r="AR29" s="5"/>
-      <c r="AS29" s="5"/>
-      <c r="AT29" s="5"/>
-      <c r="AU29" s="5"/>
-      <c r="AV29" s="5"/>
-      <c r="AW29" s="5"/>
-      <c r="AX29" s="5"/>
-      <c r="AY29" s="5"/>
+      <c r="AH29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY29" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ29" s="7" t="s">
         <v>82</v>
       </c>
       <c r="BA29" s="5"/>
       <c r="BB29" s="5"/>
     </row>
-    <row r="30" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
+    <row r="30" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="T30" s="5" t="n">
         <v>54</v>
       </c>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="5"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
+      <c r="U30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AG30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AH30" s="5"/>
-      <c r="AI30" s="5"/>
-      <c r="AJ30" s="5"/>
-      <c r="AK30" s="5"/>
-      <c r="AL30" s="5"/>
-      <c r="AM30" s="5"/>
-      <c r="AN30" s="5"/>
-      <c r="AO30" s="5"/>
-      <c r="AP30" s="5"/>
-      <c r="AQ30" s="5"/>
-      <c r="AR30" s="5"/>
-      <c r="AS30" s="5"/>
-      <c r="AT30" s="5"/>
-      <c r="AU30" s="5"/>
-      <c r="AV30" s="5"/>
-      <c r="AW30" s="5"/>
-      <c r="AX30" s="5"/>
-      <c r="AY30" s="5"/>
+      <c r="AH30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY30" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ30" s="7" t="s">
         <v>83</v>
       </c>
       <c r="BA30" s="5"/>
       <c r="BB30" s="5"/>
     </row>
-    <row r="31" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
+    <row r="31" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="S31" s="5" t="n">
         <v>54</v>
       </c>
-      <c r="T31" s="5"/>
+      <c r="T31" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="U31" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
+      <c r="V31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AG31" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AH31" s="5"/>
-      <c r="AI31" s="5"/>
-      <c r="AJ31" s="5"/>
-      <c r="AK31" s="5"/>
-      <c r="AL31" s="5"/>
-      <c r="AM31" s="5"/>
-      <c r="AN31" s="5"/>
-      <c r="AO31" s="5"/>
-      <c r="AP31" s="5"/>
-      <c r="AQ31" s="5"/>
-      <c r="AR31" s="5"/>
-      <c r="AS31" s="5"/>
-      <c r="AT31" s="5"/>
-      <c r="AU31" s="5"/>
-      <c r="AV31" s="5"/>
-      <c r="AW31" s="5"/>
-      <c r="AX31" s="5"/>
-      <c r="AY31" s="5"/>
+      <c r="AH31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY31" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ31" s="7" t="s">
         <v>84</v>
       </c>
       <c r="BA31" s="5"/>
       <c r="BB31" s="5"/>
     </row>
-    <row r="32" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
+    <row r="32" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="X32" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-      <c r="AG32" s="5"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
-      <c r="AJ32" s="5"/>
-      <c r="AK32" s="5"/>
-      <c r="AL32" s="5"/>
-      <c r="AM32" s="5"/>
-      <c r="AN32" s="5"/>
-      <c r="AO32" s="5"/>
-      <c r="AP32" s="5"/>
-      <c r="AQ32" s="5"/>
-      <c r="AR32" s="5"/>
-      <c r="AS32" s="5"/>
-      <c r="AT32" s="5"/>
-      <c r="AU32" s="5"/>
-      <c r="AV32" s="5"/>
-      <c r="AW32" s="5"/>
-      <c r="AX32" s="5"/>
-      <c r="AY32" s="5"/>
+      <c r="Y32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY32" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ32" s="7" t="s">
         <v>85</v>
       </c>
       <c r="BA32" s="5"/>
       <c r="BB32" s="5"/>
     </row>
-    <row r="33" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
+    <row r="33" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="W33" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="5"/>
-      <c r="AG33" s="5"/>
-      <c r="AH33" s="5"/>
-      <c r="AI33" s="5"/>
-      <c r="AJ33" s="5"/>
-      <c r="AK33" s="5"/>
-      <c r="AL33" s="5"/>
-      <c r="AM33" s="5"/>
-      <c r="AN33" s="5"/>
-      <c r="AO33" s="5"/>
-      <c r="AP33" s="5"/>
-      <c r="AQ33" s="5"/>
-      <c r="AR33" s="5"/>
-      <c r="AS33" s="5"/>
-      <c r="AT33" s="5"/>
-      <c r="AU33" s="5"/>
-      <c r="AV33" s="5"/>
-      <c r="AW33" s="5"/>
-      <c r="AX33" s="5"/>
-      <c r="AY33" s="5"/>
+      <c r="X33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX33" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY33" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ33" s="7" t="s">
         <v>86</v>
       </c>
       <c r="BA33" s="5"/>
       <c r="BB33" s="5"/>
     </row>
-    <row r="34" s="6" customFormat="true" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
+    <row r="34" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="V34" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="W34" s="5"/>
-      <c r="X34" s="5"/>
-      <c r="Y34" s="5"/>
-      <c r="Z34" s="5"/>
-      <c r="AA34" s="5"/>
-      <c r="AB34" s="5"/>
-      <c r="AC34" s="5"/>
-      <c r="AD34" s="5"/>
-      <c r="AE34" s="5"/>
-      <c r="AF34" s="5"/>
-      <c r="AG34" s="5"/>
-      <c r="AH34" s="5"/>
-      <c r="AI34" s="5"/>
-      <c r="AJ34" s="5"/>
-      <c r="AK34" s="5"/>
-      <c r="AL34" s="5"/>
-      <c r="AM34" s="5"/>
-      <c r="AN34" s="5"/>
-      <c r="AO34" s="5"/>
-      <c r="AP34" s="5"/>
-      <c r="AQ34" s="5"/>
-      <c r="AR34" s="5"/>
-      <c r="AS34" s="5"/>
-      <c r="AT34" s="5"/>
-      <c r="AU34" s="5"/>
-      <c r="AV34" s="5"/>
-      <c r="AW34" s="5"/>
-      <c r="AX34" s="5"/>
-      <c r="AY34" s="5"/>
+      <c r="W34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY34" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="AZ34" s="7" t="s">
         <v>87</v>
       </c>
       <c r="BA34" s="5"/>
       <c r="BB34" s="5"/>
     </row>
-    <row r="35" s="6" customFormat="true" ht="195.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>71</v>
+    <row r="35" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>71</v>
@@ -5375,7 +6330,7 @@
       <c r="BA35" s="5"/>
       <c r="BB35" s="5"/>
     </row>
-    <row r="36" s="6" customFormat="true" ht="195.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" s="6" customFormat="true" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -5431,7 +6386,6 @@
       <c r="BA36" s="8"/>
       <c r="BB36" s="8"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>